<commit_message>
Create import loc ebba applications script and split up import loc all script (#987)
</commit_message>
<xml_diff>
--- a/services/api-server/scripts/data/line_of_credit_all_2021_04_27.xlsx
+++ b/services/api-server/scripts/data/line_of_credit_all_2021_04_27.xlsx
@@ -476,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -545,6 +545,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -5295,11 +5313,11 @@
         <v>2955054.84</v>
       </c>
       <c r="E2" s="15"/>
-      <c r="F2" s="14">
-        <v>44286.0</v>
-      </c>
-      <c r="G2" s="14">
-        <v>44286.0</v>
+      <c r="F2" s="3">
+        <v>44287.0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>44287.0</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
@@ -14220,180 +14238,168 @@
       <c r="K74" s="15"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B75" s="25" t="s">
+      <c r="A75" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C75" s="26">
-        <v>44069.0</v>
-      </c>
-      <c r="D75" s="26">
-        <v>44071.0</v>
-      </c>
-      <c r="E75" s="27">
-        <v>20160.43</v>
-      </c>
-      <c r="F75" s="27">
-        <v>20065.2</v>
-      </c>
-      <c r="G75" s="27">
-        <v>95.23</v>
-      </c>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="27">
+      <c r="C75" s="14">
+        <v>44169.0</v>
+      </c>
+      <c r="D75" s="14">
+        <v>44169.0</v>
+      </c>
+      <c r="E75" s="15">
+        <v>43983.35</v>
+      </c>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15">
+        <v>43983.35</v>
+      </c>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15">
         <v>0.0</v>
       </c>
-      <c r="K75" s="29"/>
+      <c r="K75" s="15"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B76" s="25" t="s">
+      <c r="A76" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C76" s="26">
-        <v>44082.0</v>
-      </c>
-      <c r="D76" s="26">
-        <v>44084.0</v>
-      </c>
-      <c r="E76" s="27">
-        <v>45740.92</v>
-      </c>
-      <c r="F76" s="27">
-        <v>45326.0</v>
-      </c>
-      <c r="G76" s="27">
-        <v>414.91999999999825</v>
-      </c>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="27">
+      <c r="C76" s="14">
+        <v>44201.0</v>
+      </c>
+      <c r="D76" s="14">
+        <v>44201.0</v>
+      </c>
+      <c r="E76" s="15">
+        <v>67425.0</v>
+      </c>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15">
+        <v>67425.0</v>
+      </c>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15">
         <v>0.0</v>
       </c>
-      <c r="K76" s="29"/>
+      <c r="K76" s="15"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B77" s="25" t="s">
+      <c r="A77" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C77" s="26">
-        <v>44089.0</v>
-      </c>
-      <c r="D77" s="26">
-        <v>44091.0</v>
-      </c>
-      <c r="E77" s="27">
-        <v>128865.51</v>
-      </c>
-      <c r="F77" s="27">
-        <v>127791.2</v>
-      </c>
-      <c r="G77" s="27">
-        <v>1074.31</v>
-      </c>
-      <c r="H77" s="28"/>
-      <c r="I77" s="28"/>
-      <c r="J77" s="27">
+      <c r="C77" s="14">
+        <v>44232.0</v>
+      </c>
+      <c r="D77" s="14">
+        <v>44232.0</v>
+      </c>
+      <c r="E77" s="15">
+        <v>72451.68</v>
+      </c>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15">
+        <v>72451.68</v>
+      </c>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15">
         <v>0.0</v>
       </c>
-      <c r="K77" s="29"/>
+      <c r="K77" s="15"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B78" s="25" t="s">
+      <c r="A78" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C78" s="26">
-        <v>44105.0</v>
-      </c>
-      <c r="D78" s="26">
-        <v>44106.0</v>
-      </c>
-      <c r="E78" s="27">
-        <v>10000.0</v>
-      </c>
-      <c r="F78" s="27">
-        <v>9348.999999999998</v>
-      </c>
-      <c r="G78" s="27">
-        <v>651.0000000000014</v>
-      </c>
-      <c r="H78" s="28"/>
-      <c r="I78" s="28"/>
-      <c r="J78" s="27">
+      <c r="C78" s="14">
+        <v>44243.0</v>
+      </c>
+      <c r="D78" s="14">
+        <v>44245.0</v>
+      </c>
+      <c r="E78" s="15">
+        <v>2550000.0</v>
+      </c>
+      <c r="F78" s="15">
+        <v>2550000.0</v>
+      </c>
+      <c r="G78" s="15">
         <v>0.0</v>
       </c>
-      <c r="K78" s="29"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="K78" s="15"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B79" s="25" t="s">
+      <c r="A79" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="26">
-        <v>44111.0</v>
-      </c>
-      <c r="D79" s="26">
-        <v>44113.0</v>
-      </c>
-      <c r="E79" s="27">
-        <v>81540.93</v>
-      </c>
-      <c r="F79" s="27">
-        <v>30575.449999999993</v>
-      </c>
-      <c r="G79" s="27">
-        <v>965.48</v>
-      </c>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="27">
+      <c r="C79" s="14">
+        <v>44260.0</v>
+      </c>
+      <c r="D79" s="14">
+        <v>44260.0</v>
+      </c>
+      <c r="E79" s="15">
+        <v>71436.76000000042</v>
+      </c>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15">
+        <v>71436.76000000042</v>
+      </c>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15">
         <v>0.0</v>
       </c>
-      <c r="K79" s="30">
-        <v>50000.0</v>
-      </c>
+      <c r="K79" s="15"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B80" s="25" t="s">
+      <c r="A80" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C80" s="26">
-        <v>44123.0</v>
-      </c>
-      <c r="D80" s="26">
-        <v>44124.0</v>
-      </c>
-      <c r="E80" s="27">
-        <v>25000.0</v>
-      </c>
-      <c r="F80" s="27">
-        <v>24004.76</v>
-      </c>
-      <c r="G80" s="27">
-        <v>995.24</v>
-      </c>
-      <c r="H80" s="28"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="27">
+      <c r="C80" s="14">
+        <v>44292.0</v>
+      </c>
+      <c r="D80" s="14">
+        <v>44292.0</v>
+      </c>
+      <c r="E80" s="15">
+        <v>49299.97</v>
+      </c>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15">
+        <v>49299.97</v>
+      </c>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15">
         <v>0.0</v>
       </c>
-      <c r="K80" s="29"/>
+      <c r="K80" s="15"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="25" t="s">
@@ -14403,19 +14409,19 @@
         <v>124</v>
       </c>
       <c r="C81" s="26">
-        <v>44125.0</v>
+        <v>44069.0</v>
       </c>
       <c r="D81" s="26">
-        <v>44127.0</v>
+        <v>44071.0</v>
       </c>
       <c r="E81" s="27">
-        <v>50000.0</v>
+        <v>20160.43</v>
       </c>
       <c r="F81" s="27">
-        <v>49713.56</v>
+        <v>20065.2</v>
       </c>
       <c r="G81" s="27">
-        <v>286.44</v>
+        <v>95.23</v>
       </c>
       <c r="H81" s="28"/>
       <c r="I81" s="28"/>
@@ -14432,17 +14438,19 @@
         <v>124</v>
       </c>
       <c r="C82" s="26">
-        <v>44140.0</v>
+        <v>44082.0</v>
       </c>
       <c r="D82" s="26">
-        <v>44140.0</v>
+        <v>44084.0</v>
       </c>
       <c r="E82" s="27">
-        <v>1139.8</v>
-      </c>
-      <c r="F82" s="28"/>
+        <v>45740.92</v>
+      </c>
+      <c r="F82" s="27">
+        <v>45326.0</v>
+      </c>
       <c r="G82" s="27">
-        <v>1139.8</v>
+        <v>414.91999999999825</v>
       </c>
       <c r="H82" s="28"/>
       <c r="I82" s="28"/>
@@ -14459,19 +14467,19 @@
         <v>124</v>
       </c>
       <c r="C83" s="26">
-        <v>44140.0</v>
+        <v>44089.0</v>
       </c>
       <c r="D83" s="26">
-        <v>44144.0</v>
+        <v>44091.0</v>
       </c>
       <c r="E83" s="27">
-        <v>86016.69</v>
+        <v>128865.51</v>
       </c>
       <c r="F83" s="27">
-        <v>84802.88</v>
+        <v>127791.2</v>
       </c>
       <c r="G83" s="27">
-        <v>1213.81</v>
+        <v>1074.31</v>
       </c>
       <c r="H83" s="28"/>
       <c r="I83" s="28"/>
@@ -14488,19 +14496,19 @@
         <v>124</v>
       </c>
       <c r="C84" s="26">
-        <v>44152.0</v>
+        <v>44105.0</v>
       </c>
       <c r="D84" s="26">
-        <v>44154.0</v>
+        <v>44106.0</v>
       </c>
       <c r="E84" s="27">
-        <v>40254.74</v>
+        <v>10000.0</v>
       </c>
       <c r="F84" s="27">
-        <v>39298.38</v>
+        <v>9348.999999999998</v>
       </c>
       <c r="G84" s="27">
-        <v>956.36</v>
+        <v>651.0000000000014</v>
       </c>
       <c r="H84" s="28"/>
       <c r="I84" s="28"/>
@@ -14517,19 +14525,19 @@
         <v>124</v>
       </c>
       <c r="C85" s="26">
-        <v>44159.0</v>
+        <v>44111.0</v>
       </c>
       <c r="D85" s="26">
-        <v>44162.0</v>
+        <v>44113.0</v>
       </c>
       <c r="E85" s="27">
-        <v>54609.78</v>
+        <v>81540.93</v>
       </c>
       <c r="F85" s="27">
-        <v>28672.51</v>
+        <v>30575.449999999993</v>
       </c>
       <c r="G85" s="27">
-        <v>937.27</v>
+        <v>965.48</v>
       </c>
       <c r="H85" s="28"/>
       <c r="I85" s="28"/>
@@ -14537,7 +14545,7 @@
         <v>0.0</v>
       </c>
       <c r="K85" s="30">
-        <v>25000.0</v>
+        <v>50000.0</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -14548,28 +14556,26 @@
         <v>124</v>
       </c>
       <c r="C86" s="26">
-        <v>44166.0</v>
+        <v>44123.0</v>
       </c>
       <c r="D86" s="26">
-        <v>44168.0</v>
+        <v>44124.0</v>
       </c>
       <c r="E86" s="27">
-        <v>51302.4</v>
+        <v>25000.0</v>
       </c>
       <c r="F86" s="27">
-        <v>41021.21</v>
+        <v>24004.76</v>
       </c>
       <c r="G86" s="27">
-        <v>281.19</v>
+        <v>995.24</v>
       </c>
       <c r="H86" s="28"/>
       <c r="I86" s="28"/>
       <c r="J86" s="27">
         <v>0.0</v>
       </c>
-      <c r="K86" s="30">
-        <v>10000.0</v>
-      </c>
+      <c r="K86" s="29"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="25" t="s">
@@ -14579,28 +14585,26 @@
         <v>124</v>
       </c>
       <c r="C87" s="26">
-        <v>44173.0</v>
+        <v>44125.0</v>
       </c>
       <c r="D87" s="26">
-        <v>44175.0</v>
+        <v>44127.0</v>
       </c>
       <c r="E87" s="27">
-        <v>52584.96</v>
+        <v>50000.0</v>
       </c>
       <c r="F87" s="27">
-        <v>16719.33</v>
+        <v>49713.56</v>
       </c>
       <c r="G87" s="27">
-        <v>865.63</v>
+        <v>286.44</v>
       </c>
       <c r="H87" s="28"/>
       <c r="I87" s="28"/>
       <c r="J87" s="27">
         <v>0.0</v>
       </c>
-      <c r="K87" s="30">
-        <v>35000.0</v>
-      </c>
+      <c r="K87" s="29"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="25" t="s">
@@ -14610,59 +14614,53 @@
         <v>124</v>
       </c>
       <c r="C88" s="26">
-        <v>44182.0</v>
+        <v>44140.0</v>
       </c>
       <c r="D88" s="26">
-        <v>44186.0</v>
+        <v>44140.0</v>
       </c>
       <c r="E88" s="27">
-        <v>141768.9</v>
-      </c>
-      <c r="F88" s="27">
-        <v>91768.9</v>
-      </c>
+        <v>1139.8</v>
+      </c>
+      <c r="F88" s="28"/>
       <c r="G88" s="27">
-        <v>0.0</v>
+        <v>1139.8</v>
       </c>
       <c r="H88" s="28"/>
       <c r="I88" s="28"/>
       <c r="J88" s="27">
         <v>0.0</v>
       </c>
-      <c r="K88" s="30">
-        <v>50000.0</v>
-      </c>
+      <c r="K88" s="29"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B89" s="25" t="s">
+      <c r="A89" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B89" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="C89" s="26">
-        <v>44187.0</v>
-      </c>
-      <c r="D89" s="26">
-        <v>44189.0</v>
-      </c>
-      <c r="E89" s="27">
-        <v>92498.15</v>
-      </c>
-      <c r="F89" s="27">
-        <v>72498.15</v>
-      </c>
-      <c r="G89" s="27">
+      <c r="C89" s="32">
+        <v>44140.0</v>
+      </c>
+      <c r="D89" s="32">
+        <v>44144.0</v>
+      </c>
+      <c r="E89" s="33">
+        <v>86016.67</v>
+      </c>
+      <c r="F89" s="34">
+        <v>84802.88</v>
+      </c>
+      <c r="G89" s="33">
+        <v>1213.79</v>
+      </c>
+      <c r="H89" s="35"/>
+      <c r="I89" s="35"/>
+      <c r="J89" s="34">
         <v>0.0</v>
       </c>
-      <c r="H89" s="28"/>
-      <c r="I89" s="28"/>
-      <c r="J89" s="27">
-        <v>0.0</v>
-      </c>
-      <c r="K89" s="30">
-        <v>20000.0</v>
-      </c>
+      <c r="K89" s="36"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="25" t="s">
@@ -14672,19 +14670,19 @@
         <v>124</v>
       </c>
       <c r="C90" s="26">
-        <v>44194.0</v>
+        <v>44152.0</v>
       </c>
       <c r="D90" s="26">
-        <v>44196.0</v>
+        <v>44154.0</v>
       </c>
       <c r="E90" s="27">
-        <v>58447.15</v>
+        <v>40254.74</v>
       </c>
       <c r="F90" s="27">
-        <v>58447.15</v>
+        <v>39298.38</v>
       </c>
       <c r="G90" s="27">
-        <v>0.0</v>
+        <v>956.36</v>
       </c>
       <c r="H90" s="28"/>
       <c r="I90" s="28"/>
@@ -14701,19 +14699,19 @@
         <v>124</v>
       </c>
       <c r="C91" s="26">
-        <v>44201.0</v>
+        <v>44159.0</v>
       </c>
       <c r="D91" s="26">
-        <v>44202.0</v>
+        <v>44162.0</v>
       </c>
       <c r="E91" s="27">
-        <v>104067.72</v>
+        <v>54609.78</v>
       </c>
       <c r="F91" s="27">
-        <v>0.0</v>
+        <v>28672.51</v>
       </c>
       <c r="G91" s="27">
-        <v>0.0</v>
+        <v>937.27</v>
       </c>
       <c r="H91" s="28"/>
       <c r="I91" s="28"/>
@@ -14721,7 +14719,7 @@
         <v>0.0</v>
       </c>
       <c r="K91" s="30">
-        <v>104067.72</v>
+        <v>25000.0</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -14732,26 +14730,28 @@
         <v>124</v>
       </c>
       <c r="C92" s="26">
-        <v>44201.0</v>
+        <v>44166.0</v>
       </c>
       <c r="D92" s="26">
-        <v>44203.0</v>
+        <v>44168.0</v>
       </c>
       <c r="E92" s="27">
-        <v>70092.67</v>
+        <v>51302.4</v>
       </c>
       <c r="F92" s="27">
-        <v>66555.24</v>
+        <v>41021.21</v>
       </c>
       <c r="G92" s="27">
-        <v>3537.429999999993</v>
+        <v>281.19</v>
       </c>
       <c r="H92" s="28"/>
       <c r="I92" s="28"/>
       <c r="J92" s="27">
         <v>0.0</v>
       </c>
-      <c r="K92" s="29"/>
+      <c r="K92" s="30">
+        <v>10000.0</v>
+      </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="25" t="s">
@@ -14761,26 +14761,28 @@
         <v>124</v>
       </c>
       <c r="C93" s="26">
-        <v>44215.0</v>
+        <v>44173.0</v>
       </c>
       <c r="D93" s="26">
-        <v>44217.0</v>
+        <v>44175.0</v>
       </c>
       <c r="E93" s="27">
-        <v>34427.17</v>
+        <v>52584.96</v>
       </c>
       <c r="F93" s="27">
-        <v>34427.17</v>
+        <v>16719.33</v>
       </c>
       <c r="G93" s="27">
-        <v>0.0</v>
+        <v>865.63</v>
       </c>
       <c r="H93" s="28"/>
       <c r="I93" s="28"/>
       <c r="J93" s="27">
         <v>0.0</v>
       </c>
-      <c r="K93" s="29"/>
+      <c r="K93" s="30">
+        <v>35000.0</v>
+      </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="25" t="s">
@@ -14790,16 +14792,16 @@
         <v>124</v>
       </c>
       <c r="C94" s="26">
-        <v>44225.0</v>
+        <v>44182.0</v>
       </c>
       <c r="D94" s="26">
-        <v>44229.0</v>
+        <v>44186.0</v>
       </c>
       <c r="E94" s="27">
-        <v>309586.29</v>
+        <v>141768.9</v>
       </c>
       <c r="F94" s="27">
-        <v>309586.29</v>
+        <v>91768.9</v>
       </c>
       <c r="G94" s="27">
         <v>0.0</v>
@@ -14809,7 +14811,9 @@
       <c r="J94" s="27">
         <v>0.0</v>
       </c>
-      <c r="K94" s="29"/>
+      <c r="K94" s="30">
+        <v>50000.0</v>
+      </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="25" t="s">
@@ -14819,24 +14823,28 @@
         <v>124</v>
       </c>
       <c r="C95" s="26">
-        <v>44232.0</v>
+        <v>44187.0</v>
       </c>
       <c r="D95" s="26">
-        <v>44232.0</v>
+        <v>44189.0</v>
       </c>
       <c r="E95" s="27">
-        <v>3663.13</v>
-      </c>
-      <c r="F95" s="28"/>
+        <v>92498.15</v>
+      </c>
+      <c r="F95" s="27">
+        <v>72498.15</v>
+      </c>
       <c r="G95" s="27">
-        <v>3663.13</v>
+        <v>0.0</v>
       </c>
       <c r="H95" s="28"/>
       <c r="I95" s="28"/>
       <c r="J95" s="27">
         <v>0.0</v>
       </c>
-      <c r="K95" s="29"/>
+      <c r="K95" s="30">
+        <v>20000.0</v>
+      </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="25" t="s">
@@ -14846,16 +14854,16 @@
         <v>124</v>
       </c>
       <c r="C96" s="26">
-        <v>44243.0</v>
+        <v>44194.0</v>
       </c>
       <c r="D96" s="26">
-        <v>44245.0</v>
+        <v>44196.0</v>
       </c>
       <c r="E96" s="27">
-        <v>75354.84</v>
+        <v>58447.15</v>
       </c>
       <c r="F96" s="27">
-        <v>75354.84</v>
+        <v>58447.15</v>
       </c>
       <c r="G96" s="27">
         <v>0.0</v>
@@ -14875,16 +14883,16 @@
         <v>124</v>
       </c>
       <c r="C97" s="26">
-        <v>44244.0</v>
+        <v>44201.0</v>
       </c>
       <c r="D97" s="26">
-        <v>44246.0</v>
+        <v>44202.0</v>
       </c>
       <c r="E97" s="27">
-        <v>36836.8</v>
+        <v>104067.72</v>
       </c>
       <c r="F97" s="27">
-        <v>36836.8</v>
+        <v>0.0</v>
       </c>
       <c r="G97" s="27">
         <v>0.0</v>
@@ -14894,7 +14902,9 @@
       <c r="J97" s="27">
         <v>0.0</v>
       </c>
-      <c r="K97" s="29"/>
+      <c r="K97" s="30">
+        <v>104067.72</v>
+      </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="25" t="s">
@@ -14904,19 +14914,19 @@
         <v>124</v>
       </c>
       <c r="C98" s="26">
-        <v>44257.0</v>
+        <v>44201.0</v>
       </c>
       <c r="D98" s="26">
-        <v>44259.0</v>
+        <v>44203.0</v>
       </c>
       <c r="E98" s="27">
-        <v>74533.42</v>
+        <v>70092.67</v>
       </c>
       <c r="F98" s="27">
-        <v>69893.59</v>
+        <v>66555.24</v>
       </c>
       <c r="G98" s="27">
-        <v>4639.83</v>
+        <v>3537.429999999993</v>
       </c>
       <c r="H98" s="28"/>
       <c r="I98" s="28"/>
@@ -14933,16 +14943,16 @@
         <v>124</v>
       </c>
       <c r="C99" s="26">
-        <v>44264.0</v>
+        <v>44215.0</v>
       </c>
       <c r="D99" s="26">
-        <v>44266.0</v>
+        <v>44217.0</v>
       </c>
       <c r="E99" s="27">
-        <v>14428.8</v>
+        <v>34427.17</v>
       </c>
       <c r="F99" s="27">
-        <v>14428.8</v>
+        <v>34427.17</v>
       </c>
       <c r="G99" s="27">
         <v>0.0</v>
@@ -14962,16 +14972,16 @@
         <v>124</v>
       </c>
       <c r="C100" s="26">
-        <v>44285.0</v>
+        <v>44225.0</v>
       </c>
       <c r="D100" s="26">
-        <v>44287.0</v>
+        <v>44229.0</v>
       </c>
       <c r="E100" s="27">
-        <v>138255.99</v>
+        <v>309586.29</v>
       </c>
       <c r="F100" s="27">
-        <v>138255.99</v>
+        <v>309586.29</v>
       </c>
       <c r="G100" s="27">
         <v>0.0</v>
@@ -14981,7 +14991,7 @@
       <c r="J100" s="27">
         <v>0.0</v>
       </c>
-      <c r="K100" s="31"/>
+      <c r="K100" s="29"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="25" t="s">
@@ -14991,26 +15001,24 @@
         <v>124</v>
       </c>
       <c r="C101" s="26">
-        <v>44287.0</v>
+        <v>44232.0</v>
       </c>
       <c r="D101" s="26">
-        <v>44287.0</v>
+        <v>44232.0</v>
       </c>
       <c r="E101" s="27">
-        <v>1040.47</v>
-      </c>
-      <c r="F101" s="27">
-        <v>1040.47</v>
-      </c>
+        <v>3663.13</v>
+      </c>
+      <c r="F101" s="28"/>
       <c r="G101" s="27">
-        <v>0.0</v>
+        <v>3663.13</v>
       </c>
       <c r="H101" s="28"/>
       <c r="I101" s="28"/>
-      <c r="J101" s="32">
+      <c r="J101" s="27">
         <v>0.0</v>
       </c>
-      <c r="K101" s="33"/>
+      <c r="K101" s="29"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="25" t="s">
@@ -15020,17 +15028,19 @@
         <v>124</v>
       </c>
       <c r="C102" s="26">
-        <v>44292.0</v>
+        <v>44243.0</v>
       </c>
       <c r="D102" s="26">
-        <v>44292.0</v>
+        <v>44245.0</v>
       </c>
       <c r="E102" s="27">
-        <v>4367.84</v>
-      </c>
-      <c r="F102" s="28"/>
+        <v>75354.84</v>
+      </c>
+      <c r="F102" s="27">
+        <v>75354.84</v>
+      </c>
       <c r="G102" s="27">
-        <v>4367.84</v>
+        <v>0.0</v>
       </c>
       <c r="H102" s="28"/>
       <c r="I102" s="28"/>
@@ -15047,16 +15057,16 @@
         <v>124</v>
       </c>
       <c r="C103" s="26">
-        <v>44292.0</v>
+        <v>44244.0</v>
       </c>
       <c r="D103" s="26">
-        <v>44294.0</v>
+        <v>44246.0</v>
       </c>
       <c r="E103" s="27">
-        <v>80509.53</v>
+        <v>36836.8</v>
       </c>
       <c r="F103" s="27">
-        <v>80509.53</v>
+        <v>36836.8</v>
       </c>
       <c r="G103" s="27">
         <v>0.0</v>
@@ -15076,19 +15086,19 @@
         <v>124</v>
       </c>
       <c r="C104" s="26">
-        <v>44299.0</v>
+        <v>44257.0</v>
       </c>
       <c r="D104" s="26">
-        <v>44301.0</v>
+        <v>44259.0</v>
       </c>
       <c r="E104" s="27">
-        <v>24373.44</v>
+        <v>74533.42</v>
       </c>
       <c r="F104" s="27">
-        <v>24373.44</v>
+        <v>69893.59</v>
       </c>
       <c r="G104" s="27">
-        <v>0.0</v>
+        <v>4639.83</v>
       </c>
       <c r="H104" s="28"/>
       <c r="I104" s="28"/>
@@ -15105,16 +15115,16 @@
         <v>124</v>
       </c>
       <c r="C105" s="26">
-        <v>44302.0</v>
+        <v>44264.0</v>
       </c>
       <c r="D105" s="26">
-        <v>44306.0</v>
+        <v>44266.0</v>
       </c>
       <c r="E105" s="27">
-        <v>5112.73</v>
+        <v>14428.8</v>
       </c>
       <c r="F105" s="27">
-        <v>5112.73</v>
+        <v>14428.8</v>
       </c>
       <c r="G105" s="27">
         <v>0.0</v>
@@ -15134,16 +15144,16 @@
         <v>124</v>
       </c>
       <c r="C106" s="26">
-        <v>44306.0</v>
+        <v>44285.0</v>
       </c>
       <c r="D106" s="26">
-        <v>44308.0</v>
+        <v>44287.0</v>
       </c>
       <c r="E106" s="27">
-        <v>46325.92</v>
+        <v>138255.99</v>
       </c>
       <c r="F106" s="27">
-        <v>22814.469999999972</v>
+        <v>138255.99</v>
       </c>
       <c r="G106" s="27">
         <v>0.0</v>
@@ -15153,204 +15163,212 @@
       <c r="J106" s="27">
         <v>0.0</v>
       </c>
-      <c r="K106" s="30">
-        <v>23511.45</v>
-      </c>
+      <c r="K106" s="37"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B107" s="34" t="s">
+      <c r="A107" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B107" s="25" t="s">
         <v>124</v>
       </c>
       <c r="C107" s="26">
-        <v>44313.0</v>
+        <v>44287.0</v>
       </c>
       <c r="D107" s="26">
-        <v>44315.0</v>
-      </c>
-      <c r="E107" s="30">
-        <v>63652.05</v>
+        <v>44287.0</v>
+      </c>
+      <c r="E107" s="27">
+        <v>1040.47</v>
       </c>
       <c r="F107" s="27">
-        <v>0.0</v>
+        <v>1040.47</v>
       </c>
       <c r="G107" s="27">
         <v>0.0</v>
       </c>
       <c r="H107" s="28"/>
       <c r="I107" s="28"/>
-      <c r="J107" s="27">
+      <c r="J107" s="38">
         <v>0.0</v>
       </c>
-      <c r="K107" s="30">
+      <c r="K107" s="39"/>
+    </row>
+    <row r="108" ht="14.25" customHeight="1">
+      <c r="A108" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C108" s="26">
+        <v>44292.0</v>
+      </c>
+      <c r="D108" s="26">
+        <v>44292.0</v>
+      </c>
+      <c r="E108" s="27">
+        <v>4367.84</v>
+      </c>
+      <c r="F108" s="28"/>
+      <c r="G108" s="27">
+        <v>4367.84</v>
+      </c>
+      <c r="H108" s="28"/>
+      <c r="I108" s="28"/>
+      <c r="J108" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K108" s="29"/>
+    </row>
+    <row r="109" ht="14.25" customHeight="1">
+      <c r="A109" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B109" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C109" s="26">
+        <v>44292.0</v>
+      </c>
+      <c r="D109" s="26">
+        <v>44294.0</v>
+      </c>
+      <c r="E109" s="27">
+        <v>80509.53</v>
+      </c>
+      <c r="F109" s="27">
+        <v>80509.53</v>
+      </c>
+      <c r="G109" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="H109" s="28"/>
+      <c r="I109" s="28"/>
+      <c r="J109" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K109" s="29"/>
+    </row>
+    <row r="110" ht="14.25" customHeight="1">
+      <c r="A110" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C110" s="26">
+        <v>44299.0</v>
+      </c>
+      <c r="D110" s="26">
+        <v>44301.0</v>
+      </c>
+      <c r="E110" s="27">
+        <v>24373.44</v>
+      </c>
+      <c r="F110" s="27">
+        <v>24373.44</v>
+      </c>
+      <c r="G110" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="H110" s="28"/>
+      <c r="I110" s="28"/>
+      <c r="J110" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K110" s="29"/>
+    </row>
+    <row r="111" ht="14.25" customHeight="1">
+      <c r="A111" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C111" s="26">
+        <v>44302.0</v>
+      </c>
+      <c r="D111" s="26">
+        <v>44306.0</v>
+      </c>
+      <c r="E111" s="27">
+        <v>5112.73</v>
+      </c>
+      <c r="F111" s="27">
+        <v>5112.73</v>
+      </c>
+      <c r="G111" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="H111" s="28"/>
+      <c r="I111" s="28"/>
+      <c r="J111" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K111" s="29"/>
+    </row>
+    <row r="112" ht="14.25" customHeight="1">
+      <c r="A112" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C112" s="26">
+        <v>44306.0</v>
+      </c>
+      <c r="D112" s="26">
+        <v>44308.0</v>
+      </c>
+      <c r="E112" s="27">
+        <v>46325.92</v>
+      </c>
+      <c r="F112" s="27">
+        <v>22814.469999999972</v>
+      </c>
+      <c r="G112" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="H112" s="28"/>
+      <c r="I112" s="28"/>
+      <c r="J112" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K112" s="30">
+        <v>23511.45</v>
+      </c>
+    </row>
+    <row r="113" ht="14.25" customHeight="1">
+      <c r="A113" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B113" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C113" s="26">
+        <v>44313.0</v>
+      </c>
+      <c r="D113" s="26">
+        <v>44315.0</v>
+      </c>
+      <c r="E113" s="30">
         <v>63652.05</v>
       </c>
-    </row>
-    <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B108" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C108" s="14">
-        <v>44169.0</v>
-      </c>
-      <c r="D108" s="14">
-        <v>44169.0</v>
-      </c>
-      <c r="E108" s="15">
-        <v>43983.35</v>
-      </c>
-      <c r="F108" s="15"/>
-      <c r="G108" s="15">
-        <v>43983.35</v>
-      </c>
-      <c r="H108" s="15"/>
-      <c r="I108" s="15"/>
-      <c r="J108" s="15">
+      <c r="F113" s="27">
         <v>0.0</v>
       </c>
-      <c r="K108" s="15"/>
-    </row>
-    <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C109" s="14">
-        <v>44201.0</v>
-      </c>
-      <c r="D109" s="14">
-        <v>44201.0</v>
-      </c>
-      <c r="E109" s="15">
-        <v>67425.0</v>
-      </c>
-      <c r="F109" s="15"/>
-      <c r="G109" s="15">
-        <v>67425.0</v>
-      </c>
-      <c r="H109" s="15"/>
-      <c r="I109" s="15"/>
-      <c r="J109" s="15">
+      <c r="G113" s="27">
         <v>0.0</v>
       </c>
-      <c r="K109" s="15"/>
-    </row>
-    <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B110" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C110" s="14">
-        <v>44232.0</v>
-      </c>
-      <c r="D110" s="14">
-        <v>44232.0</v>
-      </c>
-      <c r="E110" s="15">
-        <v>72451.68</v>
-      </c>
-      <c r="F110" s="15"/>
-      <c r="G110" s="15">
-        <v>72451.68</v>
-      </c>
-      <c r="H110" s="15"/>
-      <c r="I110" s="15"/>
-      <c r="J110" s="15">
+      <c r="H113" s="28"/>
+      <c r="I113" s="28"/>
+      <c r="J113" s="27">
         <v>0.0</v>
       </c>
-      <c r="K110" s="15"/>
-    </row>
-    <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B111" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C111" s="14">
-        <v>44243.0</v>
-      </c>
-      <c r="D111" s="14">
-        <v>44245.0</v>
-      </c>
-      <c r="E111" s="15">
-        <v>2550000.0</v>
-      </c>
-      <c r="F111" s="15">
-        <v>2550000.0</v>
-      </c>
-      <c r="G111" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="H111" s="15"/>
-      <c r="I111" s="15"/>
-      <c r="J111" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="K111" s="15"/>
-    </row>
-    <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B112" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C112" s="14">
-        <v>44260.0</v>
-      </c>
-      <c r="D112" s="14">
-        <v>44260.0</v>
-      </c>
-      <c r="E112" s="15">
-        <v>71436.76000000042</v>
-      </c>
-      <c r="F112" s="15"/>
-      <c r="G112" s="15">
-        <v>71436.76000000042</v>
-      </c>
-      <c r="H112" s="15"/>
-      <c r="I112" s="15"/>
-      <c r="J112" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="K112" s="15"/>
-    </row>
-    <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B113" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C113" s="14">
-        <v>44292.0</v>
-      </c>
-      <c r="D113" s="14">
-        <v>44292.0</v>
-      </c>
-      <c r="E113" s="15">
-        <v>49299.97</v>
-      </c>
-      <c r="F113" s="15"/>
-      <c r="G113" s="15">
-        <v>49299.97</v>
-      </c>
-      <c r="H113" s="15"/>
-      <c r="I113" s="15"/>
-      <c r="J113" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="K113" s="15"/>
+      <c r="K113" s="30">
+        <v>63652.05</v>
+      </c>
     </row>
     <row r="114" ht="14.25" customHeight="1"/>
     <row r="115" ht="14.25" customHeight="1"/>

</xml_diff>